<commit_message>
menambahkan insert ta 1
</commit_message>
<xml_diff>
--- a/template_insert.xlsx
+++ b/template_insert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\cpdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEA1BE-BBB0-4E75-A638-A6662D708FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF60691-702C-4146-AD6C-F06DEE58C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2475" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D3B5940A-76E2-4918-8F73-9BCDE34363B8}"/>
   </bookViews>
@@ -18,6 +18,8 @@
     <sheet name="Tugas Akhir 1" sheetId="3" r:id="rId3"/>
     <sheet name="Tugas Akhir 2" sheetId="4" r:id="rId4"/>
     <sheet name="Komprehensif" sheetId="5" r:id="rId5"/>
+    <sheet name="Dosen" sheetId="6" r:id="rId6"/>
+    <sheet name="Lokasi" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="134">
   <si>
     <t>npm</t>
   </si>
@@ -178,9 +180,6 @@
     <t>M Hanif Pratama</t>
   </si>
   <si>
-    <t>Putu Putra Eka Persada</t>
-  </si>
-  <si>
     <t>Laki-laki</t>
   </si>
   <si>
@@ -196,7 +195,253 @@
     <t>email4@mail.com</t>
   </si>
   <si>
-    <t>email5@mail.com</t>
+    <t>2020/2023</t>
+  </si>
+  <si>
+    <t>judul komprehensif 1</t>
+  </si>
+  <si>
+    <t>judul komprehensif 2</t>
+  </si>
+  <si>
+    <t>judul komprehensif 3</t>
+  </si>
+  <si>
+    <t>judul komprehensif 4</t>
+  </si>
+  <si>
+    <t>2020/2024</t>
+  </si>
+  <si>
+    <t>2020/2025</t>
+  </si>
+  <si>
+    <t>2020/2026</t>
+  </si>
+  <si>
+    <t>3.88</t>
+  </si>
+  <si>
+    <t>3.89</t>
+  </si>
+  <si>
+    <t>3.90</t>
+  </si>
+  <si>
+    <t>3.91</t>
+  </si>
+  <si>
+    <t>ba/12345</t>
+  </si>
+  <si>
+    <t>ba/12346</t>
+  </si>
+  <si>
+    <t>ba/12347</t>
+  </si>
+  <si>
+    <t>ba/12348</t>
+  </si>
+  <si>
+    <t>https://vclass.unila.ac.id/user/policy.php</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>Alex Tatang</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Dosen</t>
+  </si>
+  <si>
+    <t>Mulyono, S.Si., M.Si., Ph.D.</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Hardoko Insan Qudus, M.S</t>
+  </si>
+  <si>
+    <t>Dr. Dra. Ilim, M.S.</t>
+  </si>
+  <si>
+    <t>Prof . Dr. Buhani, M.Si.</t>
+  </si>
+  <si>
+    <t>Prof. Ir. Suharso, S.Si., Ph.D.</t>
+  </si>
+  <si>
+    <t>Dr. Agung Abadi Kiswandono, S.Si., M.Sc.</t>
+  </si>
+  <si>
+    <t>Dr. Rinawati, Ph.D, S.Si, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Dian Herasari, M.Si.</t>
+  </si>
+  <si>
+    <t>Dr. Eng. Heri Satria, S.Si., M.Si.</t>
+  </si>
+  <si>
+    <t>Dr. Sonny Widiarto, S.Si., M.Sc.</t>
+  </si>
+  <si>
+    <t>Dr. Mita Rilyanti, S.Si., M.Si.</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Kamisah Delilawati Pandiangan, S.Si., M.Si.</t>
+  </si>
+  <si>
+    <t>Syaiful Bahri, S.Si, M.Si</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Noviany, S.Si., M.Si</t>
+  </si>
+  <si>
+    <t>Diky Hidayat, S.Si., M.Sc.</t>
+  </si>
+  <si>
+    <t>Dr. Eng. Suripto Dwi Yuwono, S.Si., M.T.</t>
+  </si>
+  <si>
+    <t>Dr. Yuli Ambarwati, S.Si, M.Si.</t>
+  </si>
+  <si>
+    <t>Dr. Nurhasanah, S.Si, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Ni Luh Gede Ratna Juliasih, S.Si., M.Si.</t>
+  </si>
+  <si>
+    <t>Dian Septiani Pratama, S.Si., M.Si.</t>
+  </si>
+  <si>
+    <t>Devi Nur Anisa, S.Pd., M.Sc</t>
+  </si>
+  <si>
+    <t>Hapin Afriyani, S.Si., M.Si.</t>
+  </si>
+  <si>
+    <t>Prof. Dr., Ir. Yandri A.S., M.S.</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Tati Suhartati, M.S.</t>
+  </si>
+  <si>
+    <t>Prof. Wasinton Simanjuntak, M.Sc., Ph.D.</t>
+  </si>
+  <si>
+    <t>Prof. Rudy T. Mangapul Situmeang, M.Sc., Ph.D.</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Sutopo Hadi, S.Si, M.Sc.</t>
+  </si>
+  <si>
+    <t>Prof. Drs. John Hendri,, M.S., Ph.D.</t>
+  </si>
+  <si>
+    <t>Prof. Andi Setiawan, M.Sc., Ph.D</t>
+  </si>
+  <si>
+    <t>Dra. Aspita Laila, M.S.</t>
+  </si>
+  <si>
+    <t>Dr. Zipora Sembiring, M.Si, Dra.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1W5o7PNd-HX1NsRHqs3Rror0y7U8s3GJD/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Genap</t>
+  </si>
+  <si>
+    <t>Ganjil</t>
+  </si>
+  <si>
+    <t>eyJpdiI6InNhV0FIOU8wT21VQWEyS2QzSWZmb3c9PSIsInZhbHVlIjoiMXpmWU1qK0ZxZjdCRGV4bFB0cy90dz09IiwibWFjIjoiMTY0ZWJjZTA2NDA2YWY5N2JiODNjYmVlMjZmYmViNDhlMGIxYmMzMGY2MGE3YjRkNTdkOThhNmRkZTM0OGI5YSIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6Imh0RVhtdit0OHRQcFF5QUtVdkRIVXc9PSIsInZhbHVlIjoiSHZ5NWcxT1BtSGpXNjFRQ2IrV1I1QT09IiwibWFjIjoiZTVkMjBhY2ZlMGYzMzg5MGI1ZTNjMjA1N2QwMDQ4MWU4NDA0ODY0MmMxMTBiMGRhZTgxNGQ4OTA5NDhmZTQ3ZSIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IjZsNkQzT3YrbEZaak5TelZGMDlNSHc9PSIsInZhbHVlIjoiTGVmeFRCVXY0TjQzd3pOS2dseTZnUT09IiwibWFjIjoiYjE5ZmI5NmI3MTg1ZWZkYmYyMGI2MTFlOTM2ZjIyZjJmYjMxMmIzYjhmZTE5Njg0MDBlNWFkOGNmYjliN2Y1NyIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IkVVNEF2YWwzM3RYdXNWckVGbW9jRWc9PSIsInZhbHVlIjoiRThkU1BhK3EwT1ZaZkRJTzBrRzdCUT09IiwibWFjIjoiYTdjNzViMzUxYjNkYjUyZDEzNmI3NWYwNmE0MGMzZmQ4ZWMxYzc5MTI5OTlmMjgxMzI4M2RjNmIyZDhmY2Q5YiIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6ImdIVGlLSk5IV0pkQnFCb25CdVUwdHc9PSIsInZhbHVlIjoieGtPeFB4OFlHUmdxNmU2eG84dUt3dz09IiwibWFjIjoiODIzOWYyNjg0MmYwYzBlOWU4OTM5YTk1MGNlMmYyYmZmNjM5MGZkYWFjNzFlZDc5YTQ0ZWZlMDRjOTVlZDNiMCIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IjVSNmRLcTExb3A1MGZVT1hibENaWUE9PSIsInZhbHVlIjoiT2pWQ1FSc0pJWmV6THdKYzJ5cTExUT09IiwibWFjIjoiZmIwYWNiZjhiNDMzOTAxZmFjNzI1ZTUyYzMyNmMzOTFjZTY2OWI3ZWNiNjdhY2FjMjc0ZGExNmY3ZjYwNDAwMyIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IngweUNwSGQyL2V0cnBYSWg2eXQ1T0E9PSIsInZhbHVlIjoiM21peEsvOVQ5eGxySDNDNkVwMmpCUT09IiwibWFjIjoiYzkxYjY5YjAxOTJkZDA1NmI3MzNkNWQ0OWMwOTUzOWZkZDQ5N2Y4NmVjNzg0Y2ZkMmM0MTBjNjg1OWQ1Y2NjOCIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IjBDM21wQlozVndJMmlzeWIwRTBPckE9PSIsInZhbHVlIjoiTXBCcjNyMzFEeTlJNGVrSU1SR215UT09IiwibWFjIjoiNzZkMDc1ZGY4Nzk4MjIyZDczNTg4MmRmMjQxZTA5NmZjNzFlYWMwMDZjN2U5NjZmYTgyYTIxZDU1OTdmNjkxMiIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IktGWjdUWEJVaWhTUDZBdUViZW5pM3c9PSIsInZhbHVlIjoiSlNPaldrSi9Seml5Ti9OdVpjSGQzUT09IiwibWFjIjoiMzhkYjllN2I1NGRmMjdlODY1MTFlYmEzODEyMWE5NWIxMGQwYjZjY2Y5MzdjYWM1ZmUxNTJiZWRlMzQ1NmFlYiIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IkNaaFF0TXM5RUo2MUdvZjBWRlkreUE9PSIsInZhbHVlIjoiK2pnTVBadTQxOThoRGJuMGN0THQvUT09IiwibWFjIjoiNTM3YzgzNzg2MGM0Zjk0NjJhNjI3NmJhNzliNmM4MzRjMTZmY2QyMWExYTA2N2Q0YmRlNWY4YzYwZThlMTE0NCIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6Imwrc0IvT0J3QSs1LzNjZnBEZWJvcXc9PSIsInZhbHVlIjoiNldndU11bU0yaVNsNG1BRlhOUWVrZz09IiwibWFjIjoiNTYyNjAxMjAyNmNhNzZjMmU0YTI4ZjBlMTQxNTE0NmQwNzk4MTdkMDRkYmMyMDMzYjZhYjRmYmM3YWNlZTRiZCIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>eyJpdiI6IjRDelhnTjY0UnVCZkxwL2h4WVhBYUE9PSIsInZhbHVlIjoiY3E0M1RvUGRhVTQ5dm9ZT3J4K0Vadz09IiwibWFjIjoiZTUyMmQ1ZWQwZjNjY2NiM2M4YjBkY2ZhOTQzYzc0YTliNGEyOGI2YTE0OGQwZWFjNTE4Mjg3NTRiZDA3YWZlOSIsInRhZyI6IiJ9</t>
+  </si>
+  <si>
+    <t>Ruang Biokimia Lt-1</t>
+  </si>
+  <si>
+    <t>Ruang Biokimia Lt.Dasar</t>
+  </si>
+  <si>
+    <t>Ruang SEC</t>
+  </si>
+  <si>
+    <t>Ruang Sidang Pasca FMIPA Lt-2</t>
+  </si>
+  <si>
+    <t>Ruang Diskusi Pascasarjana FMIPA Lt-1</t>
+  </si>
+  <si>
+    <t>Ruang Kelas Pascasarjana Lt-3 R1</t>
+  </si>
+  <si>
+    <t>Ruang Kelas Pascasarjana Lt-3 R2</t>
+  </si>
+  <si>
+    <t>Ruang Kelas Pascasarjana Lt-3 R3</t>
+  </si>
+  <si>
+    <t>Ruang Diskusi Pascasarjana FMIPA Lt-2</t>
+  </si>
+  <si>
+    <t>DKN Lt-3B</t>
+  </si>
+  <si>
+    <t>DKN Lt-4A</t>
+  </si>
+  <si>
+    <t>Ruang Diskusi Lt-3</t>
+  </si>
+  <si>
+    <t>Semester</t>
   </si>
 </sst>
 </file>
@@ -206,7 +451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +480,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -257,12 +508,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,7 +834,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +883,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4">
         <v>45240</v>
@@ -642,10 +895,10 @@
         <v>2020</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="H2" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -656,7 +909,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4">
         <v>45241</v>
@@ -668,10 +921,10 @@
         <v>2020</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -682,7 +935,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4">
         <v>45242</v>
@@ -694,10 +947,10 @@
         <v>2020</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -708,7 +961,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4">
         <v>45243</v>
@@ -720,49 +973,44 @@
         <v>2020</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2057051016</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45244</v>
-      </c>
-      <c r="E6" s="4">
-        <v>45244</v>
-      </c>
-      <c r="F6">
-        <v>2020</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{77E180D1-BCC0-4504-8882-5C68E01075A5}">
+      <formula1>"Laki-laki, Perempuan"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{03776BCB-1128-4796-9B46-9A8851AC80CA}"/>
-    <hyperlink ref="C3:C6" r:id="rId2" display="email@mail.com" xr:uid="{5C168257-088C-40AB-8A93-4441CEAD41DE}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{C3561F95-575C-4D28-85E8-47D319B2540B}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{4B173231-F8A0-424D-9DBE-2345AA860B25}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{AEB69AF2-4050-4079-AFCB-DD6B4C8C91AC}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{DD9C33AC-C41C-43E9-8AC8-A685401883A9}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{C3561F95-575C-4D28-85E8-47D319B2540B}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{4B173231-F8A0-424D-9DBE-2345AA860B25}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{AEB69AF2-4050-4079-AFCB-DD6B4C8C91AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C6D7578-997F-4D0A-A0AA-DA182C5453C1}">
+          <x14:formula1>
+            <xm:f>Dosen!$A$2:$A$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -770,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B847AEB-098A-4D52-8D8C-A3DB7AEA0F11}">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,28 +1107,75 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{9B06B990-8C0F-484F-B529-7F87986966FA}">
+      <formula1>"Ganjil, Genap"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{94E4054D-BB4A-455C-9242-F91B3EEFF3D8}">
+      <formula1>"Unila, Dalam Lampung, Luar Lampung"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{946DAE10-61A0-419D-A87F-C754795EBF82}">
+          <x14:formula1>
+            <xm:f>Dosen!$A$2:$A$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>N1:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D5B3B4CB-D29D-41DE-B390-50525AD1D262}">
+          <x14:formula1>
+            <xm:f>Lokasi!$B$2/Lokasi!$B$2:$B$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>R1 R3:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A9EAFED-1A3B-4C3D-86F5-E2582B4867AA}">
+          <x14:formula1>
+            <xm:f>Lokasi!$B$2:$B$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731B70F-E533-4E4B-BECD-657A97E38751}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -888,82 +1183,375 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>201705051</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2">
+        <v>450</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4">
+        <v>45078</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>201705051</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>450</v>
+      </c>
+      <c r="H3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>45079</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" t="s">
+        <v>67</v>
+      </c>
+      <c r="U3" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>201705051</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4">
+        <v>450</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4">
+        <v>45080</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4">
+        <v>30</v>
+      </c>
+      <c r="W4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>201705051</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>450</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5">
+        <v>123457</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4">
+        <v>45081</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>66</v>
+      </c>
+      <c r="S5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5">
+        <v>55</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C712" xr:uid="{1F30B4C3-9365-4BBF-B5D8-601767621FAC}">
+      <formula1>"Genap, Ganjil"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604F258F-590F-4B7F-9DF0-536F2F7FF81A}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:V1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -971,82 +1559,385 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>201705051</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2">
+        <v>450</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4">
+        <v>45078</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V2">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>201705051</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>450</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>45079</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V3">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>201705051</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4">
+        <v>450</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4">
+        <v>45080</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V4">
+        <v>30</v>
+      </c>
+      <c r="W4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>201705051</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>450</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5">
+        <v>123457</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4">
+        <v>45081</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>66</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V5">
+        <v>55</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C112" xr:uid="{3F41744D-B655-4282-923C-638EB87D3A6B}">
+      <formula1>"Genap, Ganjil"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{6453B329-6CF7-44F0-A647-805507A372AE}"/>
+    <hyperlink ref="H3:H5" r:id="rId2" display="https://drive.google.com/file/d/1W5o7PNd-HX1NsRHqs3Rror0y7U8s3GJD/view?usp=sharing" xr:uid="{2E6AB019-2B36-459F-A4FD-F384A27C9335}"/>
+    <hyperlink ref="S2" r:id="rId3" xr:uid="{099759E7-16FD-4859-B490-C7A5A4D62D8E}"/>
+    <hyperlink ref="S3:S5" r:id="rId4" display="https://drive.google.com/file/d/1W5o7PNd-HX1NsRHqs3Rror0y7U8s3GJD/view?usp=sharing" xr:uid="{88205B87-DF44-47D5-ADF1-F53334906D45}"/>
+    <hyperlink ref="T2" r:id="rId5" xr:uid="{2C90FF5C-B403-442D-A9CD-6A1BEDC10EA8}"/>
+    <hyperlink ref="T3:T5" r:id="rId6" display="https://drive.google.com/file/d/1W5o7PNd-HX1NsRHqs3Rror0y7U8s3GJD/view?usp=sharing" xr:uid="{3C330010-35B7-480B-AF05-7D36ADF25B4A}"/>
+    <hyperlink ref="U2" r:id="rId7" xr:uid="{22DBF412-89AC-445F-95B6-2E679CC7A2C5}"/>
+    <hyperlink ref="U3:U5" r:id="rId8" display="https://drive.google.com/file/d/1W5o7PNd-HX1NsRHqs3Rror0y7U8s3GJD/view?usp=sharing" xr:uid="{3BA8E439-90A6-4560-A77B-AAA46C8D964A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EC0E8B-9546-4C36-A7FE-952F704B50EA}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,64 +1945,745 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>201705051</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2">
+        <v>450</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4">
+        <v>45078</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U2" t="s">
+        <v>106</v>
+      </c>
+      <c r="V2">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>201705051</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>450</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>45079</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V3">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>201705051</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4">
+        <v>450</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4">
+        <v>45080</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T4" t="s">
+        <v>106</v>
+      </c>
+      <c r="U4" t="s">
+        <v>106</v>
+      </c>
+      <c r="V4">
+        <v>30</v>
+      </c>
+      <c r="W4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>201705051</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>450</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5">
+        <v>123457</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4">
+        <v>45081</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>66</v>
+      </c>
+      <c r="S5" t="s">
+        <v>106</v>
+      </c>
+      <c r="T5" t="s">
+        <v>106</v>
+      </c>
+      <c r="U5" t="s">
+        <v>106</v>
+      </c>
+      <c r="V5">
+        <v>55</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{29CC56D9-D968-4E88-89ED-9649D6476FE3}">
+      <formula1>"Genap, Ganjil"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{78935B9F-2D0D-4048-BBD0-7C7B53EB88B8}"/>
+    <hyperlink ref="H3:H5" r:id="rId2" display="https://drive.google.com/file/d/1W5o7PNd-HX1NsRHqs3Rror0y7U8s3GJD/view?usp=sharing" xr:uid="{E336974A-9EEC-4C90-937D-1E93D38EB9D2}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{4A242DC9-20BD-4015-AF79-F1757BEA7CC6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE3228F-9608-4612-8CD5-20F137B0DECD}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:B32" xr:uid="{B2202C6D-EC67-4961-81DE-5FCE255D077D}">
+      <formula1>1</formula1>
+      <formula2>31</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC140168-C49E-40F3-A0E3-EEC155F5C215}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="212.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menyelesaikan import mahasiswa menggunakan excel
</commit_message>
<xml_diff>
--- a/template_insert.xlsx
+++ b/template_insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\cpdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF60691-702C-4146-AD6C-F06DEE58C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540275A8-0804-4257-945F-E12671FB67E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2475" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D3B5940A-76E2-4918-8F73-9BCDE34363B8}"/>
+    <workbookView xWindow="28680" yWindow="2475" windowWidth="20730" windowHeight="11160" xr2:uid="{D3B5940A-76E2-4918-8F73-9BCDE34363B8}"/>
   </bookViews>
   <sheets>
     <sheet name="mahasiswa" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="168">
   <si>
     <t>npm</t>
   </si>
@@ -369,6 +369,9 @@
     <t>Ganjil</t>
   </si>
   <si>
+    <t>Unila</t>
+  </si>
+  <si>
     <t>eyJpdiI6InNhV0FIOU8wT21VQWEyS2QzSWZmb3c9PSIsInZhbHVlIjoiMXpmWU1qK0ZxZjdCRGV4bFB0cy90dz09IiwibWFjIjoiMTY0ZWJjZTA2NDA2YWY5N2JiODNjYmVlMjZmYmViNDhlMGIxYmMzMGY2MGE3YjRkNTdkOThhNmRkZTM0OGI5YSIsInRhZyI6IiJ9</t>
   </si>
   <si>
@@ -442,14 +445,114 @@
   </si>
   <si>
     <t>Semester</t>
+  </si>
+  <si>
+    <t>Periode Seminar</t>
+  </si>
+  <si>
+    <t>October 2021</t>
+  </si>
+  <si>
+    <t>October 2022</t>
+  </si>
+  <si>
+    <t>October 2023</t>
+  </si>
+  <si>
+    <t>October 2024</t>
+  </si>
+  <si>
+    <t>judul kerja praktik 1</t>
+  </si>
+  <si>
+    <t>judul kerja praktik 2</t>
+  </si>
+  <si>
+    <t>judul kerja praktik 3</t>
+  </si>
+  <si>
+    <t>judul kerja praktik 4</t>
+  </si>
+  <si>
+    <t>2020/2021</t>
+  </si>
+  <si>
+    <t>2020/2022</t>
+  </si>
+  <si>
+    <t>Mitra pkl 1</t>
+  </si>
+  <si>
+    <t>Mitra pkl 2</t>
+  </si>
+  <si>
+    <t>Mitra pkl 3</t>
+  </si>
+  <si>
+    <t>Mitra pkl 4</t>
+  </si>
+  <si>
+    <t>Luar Lampung</t>
+  </si>
+  <si>
+    <t>Dalam Lampung</t>
+  </si>
+  <si>
+    <t>Januari 2023</t>
+  </si>
+  <si>
+    <t>Januari 2024</t>
+  </si>
+  <si>
+    <t>Januari 2025</t>
+  </si>
+  <si>
+    <t>Januari 2026</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Boby</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Dona</t>
+  </si>
+  <si>
+    <t>3.77</t>
+  </si>
+  <si>
+    <t>3.78</t>
+  </si>
+  <si>
+    <t>3.79</t>
+  </si>
+  <si>
+    <t>3.80</t>
+  </si>
+  <si>
+    <t>baPKL/123</t>
+  </si>
+  <si>
+    <t>baPKL/124</t>
+  </si>
+  <si>
+    <t>baPKL/125</t>
+  </si>
+  <si>
+    <t>baPKL/126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -508,14 +611,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,15 +939,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558E91BE-C6C7-4F10-9018-0DE497D0E000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCellId="3" sqref="A5:H5 H4 A4:F4 A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
@@ -853,10 +959,10 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
@@ -879,16 +985,16 @@
       <c r="A2">
         <v>2017051001</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>45240</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>45240</v>
       </c>
       <c r="F2">
@@ -897,24 +1003,24 @@
       <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2017051078</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45241</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>45241</v>
       </c>
       <c r="F3">
@@ -931,16 +1037,16 @@
       <c r="A4">
         <v>2017051021</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>45242</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>45242</v>
       </c>
       <c r="F4">
@@ -957,16 +1063,16 @@
       <c r="A5">
         <v>2017051040</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>45243</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>45243</v>
       </c>
       <c r="F5">
@@ -980,17 +1086,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{77E180D1-BCC0-4504-8882-5C68E01075A5}">
-      <formula1>"Laki-laki, Perempuan"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{03776BCB-1128-4796-9B46-9A8851AC80CA}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{C3561F95-575C-4D28-85E8-47D319B2540B}"/>
@@ -999,34 +1100,43 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C6D7578-997F-4D0A-A0AA-DA182C5453C1}">
-          <x14:formula1>
-            <xm:f>Dosen!$A$2:$A$32</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B847AEB-098A-4D52-8D8C-A3DB7AEA0F11}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="78" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="207.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -1106,7 +1216,316 @@
         <v>34</v>
       </c>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2017051001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2">
+        <v>123456</v>
+      </c>
+      <c r="J2">
+        <v>450</v>
+      </c>
+      <c r="K2">
+        <v>130</v>
+      </c>
+      <c r="L2" t="s">
+        <v>160</v>
+      </c>
+      <c r="M2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2" s="3">
+        <v>43912</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="R2" t="s">
+        <v>112</v>
+      </c>
+      <c r="S2" t="s">
+        <v>164</v>
+      </c>
+      <c r="T2">
+        <v>80</v>
+      </c>
+      <c r="U2">
+        <v>80</v>
+      </c>
+      <c r="V2">
+        <v>80</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2017051078</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3">
+        <v>123457</v>
+      </c>
+      <c r="J3">
+        <v>450</v>
+      </c>
+      <c r="K3">
+        <v>130</v>
+      </c>
+      <c r="L3" t="s">
+        <v>161</v>
+      </c>
+      <c r="M3" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3" s="3">
+        <v>43913</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="R3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" t="s">
+        <v>165</v>
+      </c>
+      <c r="T3">
+        <v>80</v>
+      </c>
+      <c r="U3">
+        <v>80</v>
+      </c>
+      <c r="V3">
+        <v>80</v>
+      </c>
+      <c r="W3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2017051021</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4">
+        <v>123458</v>
+      </c>
+      <c r="J4">
+        <v>450</v>
+      </c>
+      <c r="K4">
+        <v>130</v>
+      </c>
+      <c r="L4" t="s">
+        <v>162</v>
+      </c>
+      <c r="M4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4" s="3">
+        <v>43914</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="R4" t="s">
+        <v>113</v>
+      </c>
+      <c r="S4" t="s">
+        <v>166</v>
+      </c>
+      <c r="T4">
+        <v>80</v>
+      </c>
+      <c r="U4">
+        <v>80</v>
+      </c>
+      <c r="V4">
+        <v>80</v>
+      </c>
+      <c r="W4" t="s">
+        <v>68</v>
+      </c>
+      <c r="X4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2017051040</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5">
+        <v>123459</v>
+      </c>
+      <c r="J5">
+        <v>450</v>
+      </c>
+      <c r="K5">
+        <v>130</v>
+      </c>
+      <c r="L5" t="s">
+        <v>163</v>
+      </c>
+      <c r="M5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
+      <c r="O5" s="3">
+        <v>43915</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="R5" t="s">
+        <v>115</v>
+      </c>
+      <c r="S5" t="s">
+        <v>167</v>
+      </c>
+      <c r="T5">
+        <v>80</v>
+      </c>
+      <c r="U5">
+        <v>80</v>
+      </c>
+      <c r="V5">
+        <v>80</v>
+      </c>
+      <c r="W5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{9B06B990-8C0F-484F-B529-7F87986966FA}">
       <formula1>"Ganjil, Genap"</formula1>
@@ -1129,13 +1548,13 @@
           <x14:formula1>
             <xm:f>Lokasi!$B$2/Lokasi!$B$2:$B$13</xm:f>
           </x14:formula1>
-          <xm:sqref>R1 R3:R1048576</xm:sqref>
+          <xm:sqref>R1 R33:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A9EAFED-1A3B-4C3D-86F5-E2582B4867AA}">
           <x14:formula1>
             <xm:f>Lokasi!$B$2:$B$13</xm:f>
           </x14:formula1>
-          <xm:sqref>R2</xm:sqref>
+          <xm:sqref>R2:R32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1145,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731B70F-E533-4E4B-BECD-657A97E38751}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,26 +1575,27 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="82.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1183,70 +1603,73 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201705051</v>
       </c>
@@ -1256,47 +1679,47 @@
       <c r="C2" t="s">
         <v>107</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>130</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>59</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>450</v>
       </c>
-      <c r="H2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2">
+      <c r="I2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>4</v>
       </c>
-      <c r="M2">
+      <c r="N2" s="6">
         <v>5</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="3">
         <v>45078</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="4">
         <v>0.375</v>
       </c>
-      <c r="P2" s="5">
+      <c r="Q2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>63</v>
-      </c>
-      <c r="S2" t="s">
-        <v>67</v>
       </c>
       <c r="T2" t="s">
         <v>67</v>
@@ -1304,14 +1727,17 @@
       <c r="U2" t="s">
         <v>67</v>
       </c>
-      <c r="V2">
+      <c r="V2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2">
         <v>87</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>201705051</v>
       </c>
@@ -1321,47 +1747,47 @@
       <c r="C3" t="s">
         <v>107</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" t="s">
         <v>53</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>130</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>450</v>
       </c>
-      <c r="H3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3</v>
       </c>
-      <c r="M3">
+      <c r="N3" s="6">
         <v>6</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="3">
         <v>45079</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>64</v>
-      </c>
-      <c r="S3" t="s">
-        <v>67</v>
       </c>
       <c r="T3" t="s">
         <v>67</v>
@@ -1369,14 +1795,17 @@
       <c r="U3" t="s">
         <v>67</v>
       </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>67</v>
+      </c>
+      <c r="W3">
         <v>77</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201705051</v>
       </c>
@@ -1386,47 +1815,47 @@
       <c r="C4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>130</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>61</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>450</v>
       </c>
-      <c r="H4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="M4">
+      <c r="N4" s="6">
         <v>7</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="3">
         <v>45080</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="P4" s="5">
+      <c r="Q4" s="4">
         <v>0.5</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>65</v>
-      </c>
-      <c r="S4" t="s">
-        <v>67</v>
       </c>
       <c r="T4" t="s">
         <v>67</v>
@@ -1434,14 +1863,17 @@
       <c r="U4" t="s">
         <v>67</v>
       </c>
-      <c r="V4">
+      <c r="V4" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4">
         <v>30</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201705051</v>
       </c>
@@ -1451,50 +1883,50 @@
       <c r="C5" t="s">
         <v>108</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>130</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>62</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>450</v>
       </c>
-      <c r="H5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>72</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>123457</v>
       </c>
-      <c r="M5">
+      <c r="N5" s="6">
         <v>8</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="3">
         <v>45081</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="4">
         <v>0.5</v>
       </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>4</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>66</v>
-      </c>
-      <c r="S5" t="s">
-        <v>67</v>
       </c>
       <c r="T5" t="s">
         <v>67</v>
@@ -1502,19 +1934,31 @@
       <c r="U5" t="s">
         <v>67</v>
       </c>
-      <c r="V5">
+      <c r="V5" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5">
         <v>55</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="O6" s="3"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C712" xr:uid="{1F30B4C3-9365-4BBF-B5D8-601767621FAC}">
       <formula1>"Genap, Ganjil"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{2C77204E-1E83-422A-A724-3A6395440489}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1540,7 +1984,7 @@
     <col min="9" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -1559,7 +2003,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -1591,7 +2035,7 @@
       <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="O1" t="s">
@@ -1644,7 +2088,7 @@
       <c r="G2">
         <v>450</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I2">
@@ -1656,13 +2100,13 @@
       <c r="M2">
         <v>5</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>45078</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <v>0.375</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="Q2">
@@ -1671,13 +2115,13 @@
       <c r="R2" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="S2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>106</v>
       </c>
       <c r="V2">
@@ -1709,7 +2153,7 @@
       <c r="G3">
         <v>450</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I3">
@@ -1721,13 +2165,13 @@
       <c r="M3">
         <v>6</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>45079</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>0.45833333333333298</v>
       </c>
       <c r="Q3">
@@ -1736,13 +2180,13 @@
       <c r="R3" t="s">
         <v>64</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="U3" s="3" t="s">
+      <c r="S3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>106</v>
       </c>
       <c r="V3">
@@ -1774,7 +2218,7 @@
       <c r="G4">
         <v>450</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I4">
@@ -1786,13 +2230,13 @@
       <c r="M4">
         <v>7</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>45080</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <v>0.5</v>
       </c>
       <c r="Q4">
@@ -1801,13 +2245,13 @@
       <c r="R4" t="s">
         <v>65</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="S4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="V4">
@@ -1839,7 +2283,7 @@
       <c r="G5">
         <v>450</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I5">
@@ -1854,13 +2298,13 @@
       <c r="M5">
         <v>8</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>45081</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <v>0.5</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="4">
         <v>0.54166666666666696</v>
       </c>
       <c r="Q5">
@@ -1869,13 +2313,13 @@
       <c r="R5" t="s">
         <v>66</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="U5" s="3" t="s">
+      <c r="S5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>106</v>
       </c>
       <c r="V5">
@@ -1945,7 +2389,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -2030,7 +2474,7 @@
       <c r="G2">
         <v>450</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I2">
@@ -2042,13 +2486,13 @@
       <c r="M2">
         <v>5</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>45078</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <v>0.375</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="Q2">
@@ -2095,7 +2539,7 @@
       <c r="G3">
         <v>450</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I3">
@@ -2107,13 +2551,13 @@
       <c r="M3">
         <v>6</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>45079</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>0.45833333333333298</v>
       </c>
       <c r="Q3">
@@ -2160,7 +2604,7 @@
       <c r="G4">
         <v>450</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I4">
@@ -2172,13 +2616,13 @@
       <c r="M4">
         <v>7</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>45080</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <v>0.5</v>
       </c>
       <c r="Q4">
@@ -2187,7 +2631,7 @@
       <c r="R4" t="s">
         <v>65</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="T4" t="s">
@@ -2225,7 +2669,7 @@
       <c r="G5">
         <v>450</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I5">
@@ -2240,13 +2684,13 @@
       <c r="M5">
         <v>8</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>45081</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <v>0.5</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="4">
         <v>0.54166666666666696</v>
       </c>
       <c r="Q5">
@@ -2592,98 +3036,98 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>